<commit_message>
correção no script g19.9 e atualização da base
</commit_message>
<xml_diff>
--- a/Data/g19.9.xlsx
+++ b/Data/g19.9.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,11 +459,6 @@
           <t>Posição relativamente às demais UF</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Faltam dados para todos os Estados</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -482,12 +477,9 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>12.73287554584524</v>
+        <v>19.5367037911304</v>
       </c>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -506,12 +498,9 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>12.97489130555118</v>
+        <v>18.7691365547267</v>
       </c>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -530,12 +519,9 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>13.68232552634555</v>
+        <v>17.75241147846269</v>
       </c>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -554,12 +540,9 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>13.11379688250342</v>
+        <v>16.28100354585489</v>
       </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -578,12 +561,9 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>11.94223451277554</v>
+        <v>15.8148072839542</v>
       </c>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -602,12 +582,9 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>11.76881496409633</v>
+        <v>16.1193401823764</v>
       </c>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -626,12 +603,9 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>12.0977543223817</v>
+        <v>16.67367574713436</v>
       </c>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -650,12 +624,9 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>12.74924934636568</v>
+        <v>16.54723816555322</v>
       </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -674,12 +645,9 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>12.1377771318208</v>
+        <v>16.97629758730712</v>
       </c>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -698,22 +666,19 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>13.8307044918256</v>
+        <v>17.67162353660616</v>
       </c>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>Nordeste</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>01/01/2025</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -722,12 +687,9 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>9.474718372887331</v>
+        <v>22.34782353990431</v>
       </c>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -737,7 +699,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -746,12 +708,9 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>16.73480696636505</v>
+        <v>21.72884698728347</v>
       </c>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -761,7 +720,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -770,12 +729,9 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>16.45884553085288</v>
+        <v>19.93727375877596</v>
       </c>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -785,7 +741,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -794,12 +750,9 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>13.89967984937273</v>
+        <v>18.6593769057677</v>
       </c>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -809,7 +762,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -818,12 +771,9 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>14.76660569953508</v>
+        <v>17.92702368561801</v>
       </c>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -833,7 +783,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -842,12 +792,9 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>12.63416987646953</v>
+        <v>18.39897530445306</v>
       </c>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -857,7 +804,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -866,12 +813,9 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>12.4691647775766</v>
+        <v>18.6127220282535</v>
       </c>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -881,7 +825,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -890,12 +834,9 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>12.47276728182001</v>
+        <v>18.31537882657421</v>
       </c>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -905,7 +846,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -914,12 +855,9 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>12.57007644680532</v>
+        <v>19.71373812688735</v>
       </c>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -929,7 +867,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>01/01/2023</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -938,22 +876,19 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>12.27746737632509</v>
+        <v>21.52258603851626</v>
       </c>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Sergipe</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>01/01/2024</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -962,22 +897,21 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>13.5652723062943</v>
-      </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="b">
-        <v>0</v>
+        <v>25.89068540205256</v>
+      </c>
+      <c r="E22" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Nordeste</t>
+          <t>Sergipe</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>01/01/2025</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -986,11 +920,10 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>9.496794319864035</v>
-      </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="b">
-        <v>0</v>
+        <v>21.60748792710043</v>
+      </c>
+      <c r="E23" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="24">
@@ -1001,7 +934,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>01/01/2015</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1010,13 +943,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>15.33841275398043</v>
+        <v>18.75518027117731</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
-      </c>
-      <c r="F24" t="b">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25">
@@ -1027,7 +957,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>01/01/2016</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1036,13 +966,10 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>12.47132489276449</v>
+        <v>17.87103043104207</v>
       </c>
       <c r="E25" t="n">
-        <v>12</v>
-      </c>
-      <c r="F25" t="b">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26">
@@ -1053,7 +980,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>01/01/2017</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1062,13 +989,10 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>10.1007147584733</v>
+        <v>17.84678534778923</v>
       </c>
       <c r="E26" t="n">
-        <v>20</v>
-      </c>
-      <c r="F26" t="b">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27">
@@ -1079,7 +1003,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>01/01/2018</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1088,14 +1012,11 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>11.499762104158</v>
+        <v>18.49865452232216</v>
       </c>
       <c r="E27" t="n">
         <v>15</v>
       </c>
-      <c r="F27" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1105,7 +1026,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>01/01/2019</t>
+          <t>01/01/2021</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1114,13 +1035,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>8.308314143012621</v>
+        <v>18.6760161540917</v>
       </c>
       <c r="E28" t="n">
-        <v>22</v>
-      </c>
-      <c r="F28" t="b">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29">
@@ -1131,7 +1049,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>01/01/2022</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1140,13 +1058,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6.468216048765174</v>
+        <v>18.64892907205304</v>
       </c>
       <c r="E29" t="n">
-        <v>24</v>
-      </c>
-      <c r="F29" t="b">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30">
@@ -1157,7 +1072,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>01/01/2021</t>
+          <t>01/01/2023</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1166,13 +1081,10 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>6.200057468118876</v>
+        <v>20.33309465318489</v>
       </c>
       <c r="E30" t="n">
-        <v>24</v>
-      </c>
-      <c r="F30" t="b">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31">
@@ -1183,7 +1095,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>01/01/2022</t>
+          <t>01/01/2024</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1192,91 +1104,10 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>5.089403861161063</v>
+        <v>24.57359573685214</v>
       </c>
       <c r="E31" t="n">
-        <v>26</v>
-      </c>
-      <c r="F31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Sergipe</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>01/01/2023</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Morte no trânsito ou em decorrência dele (exceto homicídio doloso)</t>
-        </is>
-      </c>
-      <c r="D32" t="n">
-        <v>6.648580843587086</v>
-      </c>
-      <c r="E32" t="n">
-        <v>23</v>
-      </c>
-      <c r="F32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Sergipe</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>01/01/2024</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Morte no trânsito ou em decorrência dele (exceto homicídio doloso)</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>8.143716976183596</v>
-      </c>
-      <c r="E33" t="n">
-        <v>21</v>
-      </c>
-      <c r="F33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Sergipe</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>01/01/2025</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Morte no trânsito ou em decorrência dele (exceto homicídio doloso)</t>
-        </is>
-      </c>
-      <c r="D34" t="n">
-        <v>5.182588823353326</v>
-      </c>
-      <c r="E34" t="n">
-        <v>23</v>
-      </c>
-      <c r="F34" t="b">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>